<commit_message>
updated log error chart to match original study
</commit_message>
<xml_diff>
--- a/study data csvs/total.xlsx
+++ b/study data csvs/total.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Evelyn\Documents\GitHub\03-experiment\study data csvs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EA2CA9-7618-4DA2-8A18-B17C4ED098E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B3E3B9-1683-4F3C-A70C-5A4FB234E158}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{4E65F5C6-6F13-A448-B601-662B42475515}"/>
   </bookViews>
@@ -189,13 +189,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Average</a:t>
+              <a:t>Study Results</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Percent Error</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -230,63 +225,108 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.24470296960797278"/>
+          <c:y val="0.17171296296296296"/>
+          <c:w val="0.71840811579174457"/>
+          <c:h val="0.62271617089530473"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Averages</c:v>
+            <c:strRef>
+              <c:f>Comparison!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Comparison!$F$6:$F$8</c:f>
+                <c:f>Comparison!$E$2:$E$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>1.6048758972636201E-2</c:v>
+                    <c:v>0.23099876791560287</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.1410486887611394E-2</c:v>
+                    <c:v>0.24226233771840633</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.6671965533050596E-2</c:v>
+                    <c:v>0.23512944404328015</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Comparison!$E$6:$E$8</c:f>
+                <c:f>Comparison!$E$2:$E$4</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>1.142878361432414E-2</c:v>
+                    <c:v>0.23099876791560287</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.6565240133243266E-2</c:v>
+                    <c:v>0.24226233771840633</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.1969376652184996E-2</c:v>
+                    <c:v>0.23512944404328015</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -305,44 +345,46 @@
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
-          <c:cat>
-            <c:strRef>
-              <c:f>Comparison!$A$2:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Bar</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Radar</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Circular</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
+          <c:xVal>
             <c:numRef>
-              <c:f>Comparison!$B$6:$B$8</c:f>
+              <c:f>Comparison!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.3738771293480169E-2</c:v>
+                  <c:v>1.373877129348017</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8987863510427326E-2</c:v>
+                  <c:v>1.8987863510427327</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4320671092617797E-2</c:v>
+                  <c:v>2.4320671092617796</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Comparison!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D477-41DB-9094-A4C245DD2766}"/>
+              <c16:uniqueId val="{00000000-68C1-42ED-A915-C0D2F2556F37}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -354,13 +396,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="378670336"/>
-        <c:axId val="378669680"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="378670336"/>
+        <c:axId val="583630392"/>
+        <c:axId val="583634328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="583630392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -387,11 +427,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Graph</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Type</a:t>
+                  <a:t>Log Error</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -434,8 +470,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -462,137 +498,24 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="378669680"/>
+        <c:crossAx val="583634328"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="378669680"/>
+        <c:axId val="583634328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Percent Error</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="378670336"/>
+        <c:crossAx val="583630392"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -643,6 +566,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -687,7 +611,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -714,8 +638,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -816,7 +740,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -848,10 +772,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -891,22 +815,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1011,8 +936,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1144,19 +1069,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1170,6 +1096,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1193,23 +1130,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>707570</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19793</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>598683</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>128074</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>702623</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>108859</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>64293</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>100364</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{787FE616-B6BF-4DCB-BB8A-1FEE76645A7B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20963B62-7344-48D5-9A26-A7EA7D88CB12}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1228,6 +1165,265 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.012</cdr:x>
+      <cdr:y>0.33362</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.24508</cdr:x>
+      <cdr:y>0.4148</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6A20CE2-76E1-4136-87B6-BE1E3CFF379A}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="55162" y="909229"/>
+          <a:ext cx="1071717" cy="221226"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Bar Chart</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00784</cdr:x>
+      <cdr:y>0.466</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.23866</cdr:x>
+      <cdr:y>0.54717</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E45387A-A9A4-41AA-BEBC-EF31BA7A86CA}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="36052" y="1270000"/>
+          <a:ext cx="1061329" cy="221226"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Radar Chart</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00677</cdr:x>
+      <cdr:y>0.60309</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.24615</cdr:x>
+      <cdr:y>0.68427</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E45387A-A9A4-41AA-BEBC-EF31BA7A86CA}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="31135" y="1643625"/>
+          <a:ext cx="1100659" cy="221226"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Circular Barplot</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26935,7 +27131,7 @@
         <v>0.50819672131147497</v>
       </c>
       <c r="G706">
-        <f t="shared" ref="G706:G769" si="44">LOG(ABS(E706-F706)+(1/8),2)</f>
+        <f t="shared" ref="G706:G721" si="44">LOG(ABS(E706-F706)+(1/8),2)</f>
         <v>-2.9083695245344368</v>
       </c>
       <c r="H706">
@@ -50683,155 +50879,164 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E250413C-E5AF-FA47-8929-C030BAD950AF}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="H6" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
         <f>AVERAGE(Bargraph!$J$2:$J$241)</f>
         <v>1.373877129348017</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <f>STDEV(Bargraph!$J$2:$J$241)</f>
         <v>1.8258588181996851</v>
       </c>
-      <c r="D2">
-        <f>CONFIDENCE(0.05,C2,COUNT(Bargraph!$J$2:$J$241))</f>
+      <c r="E2">
+        <f>CONFIDENCE(0.05,D2,COUNT(Bargraph!$J$2:$J$241))</f>
         <v>0.23099876791560287</v>
       </c>
-      <c r="E2">
-        <f>B2-D2</f>
+      <c r="F2">
+        <f>C2-E2</f>
         <v>1.1428783614324141</v>
       </c>
-      <c r="F2">
-        <f>B2+D2</f>
+      <c r="G2">
+        <f>C2+E2</f>
         <v>1.6048758972636199</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
         <f>AVERAGE(Radar!$J$2:$J$241)</f>
         <v>1.8987863510427327</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <f>STDEV(Radar!$J$2:$J$241)</f>
         <v>1.9148882465140831</v>
       </c>
-      <c r="D3">
-        <f>CONFIDENCE(0.05,C3,COUNT(Radar!$J$2:$J$241))</f>
+      <c r="E3">
+        <f>CONFIDENCE(0.05,D3,COUNT(Radar!$J$2:$J$241))</f>
         <v>0.24226233771840633</v>
       </c>
-      <c r="E3">
-        <f>B3-D3</f>
+      <c r="F3">
+        <f>C3-E3</f>
         <v>1.6565240133243264</v>
       </c>
-      <c r="F3">
-        <f>B3+D3</f>
+      <c r="G3">
+        <f>C3+E3</f>
         <v>2.1410486887611393</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <f>AVERAGE('Circular Barplot'!$J$2:$J$241)</f>
         <v>2.4320671092617796</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <f>STDEV('Circular Barplot'!$J$2:$J$241)</f>
         <v>1.8585084790654178</v>
       </c>
-      <c r="D4">
-        <f>CONFIDENCE(0.05,C4,COUNT('Circular Barplot'!$J$2:$J$241))</f>
+      <c r="E4">
+        <f>CONFIDENCE(0.05,D4,COUNT('Circular Barplot'!$J$2:$J$241))</f>
         <v>0.23512944404328015</v>
       </c>
-      <c r="E4">
-        <f>B4-D4</f>
+      <c r="F4">
+        <f>C4-E4</f>
         <v>2.1969376652184995</v>
       </c>
-      <c r="F4">
-        <f>B4+D4</f>
+      <c r="G4">
+        <f>C4+E4</f>
         <v>2.6671965533050597</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6">
         <f>B2/100</f>
-        <v>1.3738771293480169E-2</v>
+        <v>0.03</v>
       </c>
       <c r="E6">
         <f>E2/100</f>
-        <v>1.142878361432414E-2</v>
+        <v>2.3099876791560286E-3</v>
       </c>
       <c r="F6">
         <f>F2/100</f>
-        <v>1.6048758972636201E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1.142878361432414E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7">
         <f t="shared" ref="B7:B8" si="0">B3/100</f>
-        <v>1.8987863510427326E-2</v>
+        <v>0.02</v>
       </c>
       <c r="E7">
         <f t="shared" ref="E7:F8" si="1">E3/100</f>
-        <v>1.6565240133243266E-2</v>
+        <v>2.4226233771840631E-3</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>2.1410486887611394E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1.6565240133243266E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>2.4320671092617797E-2</v>
+        <v>0.01</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>2.1969376652184996E-2</v>
+        <v>2.3512944404328016E-3</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>2.6671965533050596E-2</v>
+        <v>2.1969376652184996E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>